<commit_message>
Add updated Buddy Bass Weekly tourny data
</commit_message>
<xml_diff>
--- a/data/Buddy Bass Tournament 2020.xlsx
+++ b/data/Buddy Bass Tournament 2020.xlsx
@@ -11,17 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mh3fJhtukIBWDuomKVusIvRl7TCAg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgeXunhMeJRqsnhCG4iB/ZLyl2QlA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Bass Tournament Totals 2020</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -38,30 +35,20 @@
     <t>Big Fish (LBS)</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Totals</t>
+    <t>Avg Water Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="20.0"/>
-      <color theme="1"/>
-      <name val="Algerian"/>
-    </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -80,11 +67,6 @@
       <name val="Century Gothic"/>
     </font>
     <font>
-      <sz val="16.0"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-    </font>
-    <font>
       <sz val="14.0"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
@@ -95,8 +77,7 @@
       <name val="Century Gothic"/>
     </font>
     <font>
-      <b/>
-      <sz val="15.0"/>
+      <sz val="16.0"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
     </font>
@@ -109,13 +90,8 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
-    <border>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FFA5A5A5"/>
@@ -134,53 +110,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -408,1879 +358,1869 @@
     <col customWidth="1" min="1" max="1" width="11.29"/>
     <col customWidth="1" min="2" max="4" width="12.29"/>
     <col customWidth="1" min="5" max="5" width="25.14"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="8" width="20.86"/>
-    <col customWidth="1" min="9" max="25" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="12.29"/>
+    <col customWidth="1" min="7" max="23" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="3.0" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" ht="94.5" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" ht="3.0" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="94.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+    </row>
+    <row r="3" ht="23.25" customHeight="1">
+      <c r="A3" s="4">
+        <v>44006.0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>29.0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>49.0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>69.8</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4.32</v>
+      </c>
+      <c r="F3" s="5">
+        <v>75.2</v>
+      </c>
     </row>
     <row r="4" ht="23.25" customHeight="1">
-      <c r="A4" s="8">
-        <v>44006.0</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="4">
+        <v>44013.0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>61.0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42.2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5.26</v>
+      </c>
+      <c r="F4" s="5">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="5" ht="23.25" customHeight="1">
+      <c r="A5" s="4">
+        <v>44020.0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>26.0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>50.0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>92.2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="6" ht="23.25" customHeight="1">
+      <c r="A6" s="4">
+        <v>44027.0</v>
+      </c>
+      <c r="B6" s="5">
         <v>29.0</v>
       </c>
-      <c r="C4" s="9">
-        <v>49.0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>69.8</v>
-      </c>
-      <c r="E4" s="10">
-        <v>5.56</v>
-      </c>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" ht="23.25" customHeight="1">
-      <c r="A5" s="8">
-        <v>44013.0</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="C6" s="5">
+        <v>54.0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>90.31</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4.26</v>
+      </c>
+      <c r="F6" s="5">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="7" ht="23.25" customHeight="1">
+      <c r="A7" s="4">
+        <v>44034.0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>32.0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>48.0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>52.94</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5.36</v>
+      </c>
+      <c r="F7" s="5">
+        <v>80.4</v>
+      </c>
+    </row>
+    <row r="8" ht="23.25" customHeight="1">
+      <c r="A8" s="4">
+        <v>44041.0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>56.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>68.78</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.36</v>
+      </c>
+      <c r="F8" s="5">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="9" ht="23.25" customHeight="1">
+      <c r="A9" s="4">
+        <v>44048.0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>37.0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>71.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>65.74</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5.44</v>
+      </c>
+      <c r="F9" s="5">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="10" ht="23.25" customHeight="1">
+      <c r="A10" s="4">
+        <v>44055.0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="C10" s="6">
         <v>33.0</v>
       </c>
-      <c r="C5" s="9">
-        <v>61.0</v>
-      </c>
-      <c r="D5" s="10">
-        <v>42.2</v>
-      </c>
-      <c r="E5" s="10">
-        <v>5.2</v>
-      </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" ht="23.25" customHeight="1">
-      <c r="A6" s="8">
-        <v>44020.0</v>
-      </c>
-      <c r="B6" s="9">
-        <v>26.0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>50.0</v>
-      </c>
-      <c r="D6" s="10">
-        <v>92.2</v>
-      </c>
-      <c r="E6" s="10">
-        <v>4.9</v>
-      </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" ht="23.25" customHeight="1">
-      <c r="A7" s="8">
-        <v>44027.0</v>
-      </c>
-      <c r="B7" s="9">
-        <v>29.0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>54.0</v>
-      </c>
-      <c r="D7" s="10">
-        <v>90.31</v>
-      </c>
-      <c r="E7" s="10">
-        <v>3.42</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" ht="23.25" customHeight="1">
-      <c r="A8" s="8">
-        <v>44034.0</v>
-      </c>
-      <c r="B8" s="9">
-        <v>32.0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>48.0</v>
-      </c>
-      <c r="D8" s="10">
-        <v>52.94</v>
-      </c>
-      <c r="E8" s="10">
-        <v>5.28</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" ht="23.25" customHeight="1">
-      <c r="A9" s="8">
-        <v>44041.0</v>
-      </c>
-      <c r="B9" s="9">
-        <v>31.0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>56.0</v>
-      </c>
-      <c r="D9" s="10">
-        <v>68.78</v>
-      </c>
-      <c r="E9" s="10">
-        <v>4.52</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" ht="23.25" customHeight="1">
-      <c r="A10" s="8">
-        <v>44048.0</v>
-      </c>
-      <c r="B10" s="9">
-        <v>37.0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>71.0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>65.74</v>
-      </c>
-      <c r="E10" s="10">
-        <v>3.18</v>
-      </c>
-      <c r="F10" s="11"/>
+      <c r="D10" s="6">
+        <v>46.74</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2.34</v>
+      </c>
+      <c r="F10" s="5">
+        <v>84.6</v>
+      </c>
     </row>
     <row r="11" ht="23.25" customHeight="1">
-      <c r="A11" s="8">
-        <v>44055.0</v>
-      </c>
-      <c r="B11" s="9">
-        <v>31.0</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="A11" s="4">
+        <v>44062.0</v>
+      </c>
+      <c r="B11" s="5">
+        <v>28.0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>58.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>55.38</v>
+      </c>
+      <c r="E11" s="5">
+        <v>4.46</v>
+      </c>
+      <c r="F11" s="5">
+        <v>85.3</v>
+      </c>
+    </row>
+    <row r="12" ht="23.25" customHeight="1">
+      <c r="A12" s="4">
+        <v>44069.0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="C12" s="5">
         <v>33.0</v>
       </c>
-      <c r="D11" s="10">
-        <v>46.74</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D12" s="6">
+        <v>78.23</v>
+      </c>
+      <c r="E12" s="5">
         <v>2.84</v>
       </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" ht="23.25" customHeight="1">
-      <c r="A12" s="8">
-        <v>44062.0</v>
-      </c>
-      <c r="B12" s="9">
-        <v>28.0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>58.0</v>
-      </c>
-      <c r="D12" s="10">
-        <v>55.38</v>
-      </c>
-      <c r="E12" s="10">
-        <v>2.72</v>
-      </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="5">
+        <v>85.3</v>
+      </c>
     </row>
     <row r="13" ht="23.25" customHeight="1">
-      <c r="A13" s="8">
-        <v>44069.0</v>
-      </c>
-      <c r="B13" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="C13" s="9">
-        <v>33.0</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="A13" s="4">
+        <v>44087.0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>84.0</v>
+      </c>
+      <c r="D13" s="6">
         <v>78.23</v>
       </c>
-      <c r="E13" s="10">
-        <v>4.26</v>
-      </c>
-      <c r="F13" s="11"/>
+      <c r="E13" s="5">
+        <v>4.28</v>
+      </c>
+      <c r="F13" s="5">
+        <v>78.8</v>
+      </c>
     </row>
     <row r="14" ht="23.25" customHeight="1">
-      <c r="A14" s="8">
-        <v>44087.0</v>
-      </c>
-      <c r="B14" s="9">
-        <v>27.0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>84.0</v>
-      </c>
-      <c r="D14" s="10">
-        <v>78.23</v>
-      </c>
-      <c r="E14" s="10">
-        <v>4.26</v>
-      </c>
-      <c r="F14" s="11"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" ht="23.25" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" ht="23.25" customHeight="1">
-      <c r="A16" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17">
-        <f>SUM(C4:C13)</f>
-        <v>513</v>
-      </c>
-      <c r="D16" s="17">
-        <f>SUM(D4:D15)</f>
-        <v>740.55</v>
-      </c>
-      <c r="E16" s="17">
-        <f>AVERAGE(E4:E15)</f>
-        <v>4.194545455</v>
-      </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" ht="23.25" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" ht="23.25" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="11"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="11"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="11"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="11"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="11"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="11"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="11"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="11"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="11"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="11"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="11"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="11"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="11"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="11"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="11"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="11"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="11"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="11"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="11"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="11"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="11"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="11"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="11"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="11"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="11"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="11"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="11"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="11"/>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="11"/>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="11"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="11"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
-      <c r="F126" s="11"/>
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="11"/>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="11"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="11"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="11"/>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11"/>
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="11"/>
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="11"/>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="11"/>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
-      <c r="F133" s="11"/>
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="11"/>
-      <c r="B134" s="11"/>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11"/>
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
-      <c r="E135" s="11"/>
-      <c r="F135" s="11"/>
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="A136" s="11"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="11"/>
-      <c r="D136" s="11"/>
-      <c r="E136" s="11"/>
-      <c r="F136" s="11"/>
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="11"/>
-      <c r="B137" s="11"/>
-      <c r="C137" s="11"/>
-      <c r="D137" s="11"/>
-      <c r="E137" s="11"/>
-      <c r="F137" s="11"/>
+      <c r="A137" s="7"/>
+      <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="11"/>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="7"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="7"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" s="11"/>
-      <c r="B139" s="11"/>
-      <c r="C139" s="11"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
-      <c r="F139" s="11"/>
+      <c r="A139" s="7"/>
+      <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
-      <c r="F140" s="11"/>
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="11"/>
-      <c r="B141" s="11"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
-      <c r="F141" s="11"/>
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+      <c r="C141" s="7"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" s="11"/>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
-      <c r="D142" s="11"/>
-      <c r="E142" s="11"/>
-      <c r="F142" s="11"/>
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="7"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+      <c r="F142" s="7"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" s="11"/>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
+      <c r="A143" s="7"/>
+      <c r="B143" s="7"/>
+      <c r="C143" s="7"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" s="11"/>
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
-      <c r="F144" s="11"/>
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="7"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" s="11"/>
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
+      <c r="A145" s="7"/>
+      <c r="B145" s="7"/>
+      <c r="C145" s="7"/>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" s="11"/>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
+      <c r="A146" s="7"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="7"/>
+      <c r="D146" s="7"/>
+      <c r="E146" s="7"/>
+      <c r="F146" s="7"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" s="11"/>
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
+      <c r="A147" s="7"/>
+      <c r="B147" s="7"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="11"/>
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="11"/>
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="11"/>
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="A151" s="7"/>
+      <c r="B151" s="7"/>
+      <c r="C151" s="7"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="11"/>
-      <c r="B152" s="11"/>
-      <c r="C152" s="11"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="11"/>
-      <c r="F152" s="11"/>
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="11"/>
-      <c r="B153" s="11"/>
-      <c r="C153" s="11"/>
-      <c r="D153" s="11"/>
-      <c r="E153" s="11"/>
-      <c r="F153" s="11"/>
+      <c r="A153" s="7"/>
+      <c r="B153" s="7"/>
+      <c r="C153" s="7"/>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="11"/>
-      <c r="B154" s="11"/>
-      <c r="C154" s="11"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="11"/>
-      <c r="F154" s="11"/>
+      <c r="A154" s="7"/>
+      <c r="B154" s="7"/>
+      <c r="C154" s="7"/>
+      <c r="D154" s="7"/>
+      <c r="E154" s="7"/>
+      <c r="F154" s="7"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="11"/>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
-      <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
+      <c r="A155" s="7"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="11"/>
-      <c r="B156" s="11"/>
-      <c r="C156" s="11"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="7"/>
+      <c r="D156" s="7"/>
+      <c r="E156" s="7"/>
+      <c r="F156" s="7"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="11"/>
-      <c r="B157" s="11"/>
-      <c r="C157" s="11"/>
-      <c r="D157" s="11"/>
-      <c r="E157" s="11"/>
-      <c r="F157" s="11"/>
+      <c r="A157" s="7"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="7"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="11"/>
-      <c r="B158" s="11"/>
-      <c r="C158" s="11"/>
-      <c r="D158" s="11"/>
-      <c r="E158" s="11"/>
-      <c r="F158" s="11"/>
+      <c r="A158" s="7"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="7"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+      <c r="F158" s="7"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="11"/>
-      <c r="B159" s="11"/>
-      <c r="C159" s="11"/>
-      <c r="D159" s="11"/>
-      <c r="E159" s="11"/>
-      <c r="F159" s="11"/>
+      <c r="A159" s="7"/>
+      <c r="B159" s="7"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="11"/>
-      <c r="B160" s="11"/>
-      <c r="C160" s="11"/>
-      <c r="D160" s="11"/>
-      <c r="E160" s="11"/>
-      <c r="F160" s="11"/>
+      <c r="A160" s="7"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" s="11"/>
-      <c r="B161" s="11"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
-      <c r="F161" s="11"/>
+      <c r="A161" s="7"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" s="11"/>
-      <c r="B162" s="11"/>
-      <c r="C162" s="11"/>
-      <c r="D162" s="11"/>
-      <c r="E162" s="11"/>
-      <c r="F162" s="11"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="7"/>
+      <c r="D162" s="7"/>
+      <c r="E162" s="7"/>
+      <c r="F162" s="7"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
-      <c r="A163" s="11"/>
-      <c r="B163" s="11"/>
-      <c r="C163" s="11"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="11"/>
-      <c r="F163" s="11"/>
+      <c r="A163" s="7"/>
+      <c r="B163" s="7"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="A164" s="11"/>
-      <c r="B164" s="11"/>
-      <c r="C164" s="11"/>
-      <c r="D164" s="11"/>
-      <c r="E164" s="11"/>
-      <c r="F164" s="11"/>
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="7"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
+      <c r="F164" s="7"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
-      <c r="A165" s="11"/>
-      <c r="B165" s="11"/>
-      <c r="C165" s="11"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="11"/>
-      <c r="F165" s="11"/>
+      <c r="A165" s="7"/>
+      <c r="B165" s="7"/>
+      <c r="C165" s="7"/>
+      <c r="D165" s="7"/>
+      <c r="E165" s="7"/>
+      <c r="F165" s="7"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="A166" s="11"/>
-      <c r="B166" s="11"/>
-      <c r="C166" s="11"/>
-      <c r="D166" s="11"/>
-      <c r="E166" s="11"/>
-      <c r="F166" s="11"/>
+      <c r="A166" s="7"/>
+      <c r="B166" s="7"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
+      <c r="F166" s="7"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="A167" s="11"/>
-      <c r="B167" s="11"/>
-      <c r="C167" s="11"/>
-      <c r="D167" s="11"/>
-      <c r="E167" s="11"/>
-      <c r="F167" s="11"/>
+      <c r="A167" s="7"/>
+      <c r="B167" s="7"/>
+      <c r="C167" s="7"/>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7"/>
+      <c r="F167" s="7"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="A168" s="11"/>
-      <c r="B168" s="11"/>
-      <c r="C168" s="11"/>
-      <c r="D168" s="11"/>
-      <c r="E168" s="11"/>
-      <c r="F168" s="11"/>
+      <c r="A168" s="7"/>
+      <c r="B168" s="7"/>
+      <c r="C168" s="7"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
+      <c r="F168" s="7"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
-      <c r="A169" s="11"/>
-      <c r="B169" s="11"/>
-      <c r="C169" s="11"/>
-      <c r="D169" s="11"/>
-      <c r="E169" s="11"/>
-      <c r="F169" s="11"/>
+      <c r="A169" s="7"/>
+      <c r="B169" s="7"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
+      <c r="F169" s="7"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="11"/>
-      <c r="B170" s="11"/>
-      <c r="C170" s="11"/>
-      <c r="D170" s="11"/>
-      <c r="E170" s="11"/>
-      <c r="F170" s="11"/>
+      <c r="A170" s="7"/>
+      <c r="B170" s="7"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="7"/>
+      <c r="E170" s="7"/>
+      <c r="F170" s="7"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
-      <c r="A171" s="11"/>
-      <c r="B171" s="11"/>
-      <c r="C171" s="11"/>
-      <c r="D171" s="11"/>
-      <c r="E171" s="11"/>
-      <c r="F171" s="11"/>
+      <c r="A171" s="7"/>
+      <c r="B171" s="7"/>
+      <c r="C171" s="7"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
+      <c r="F171" s="7"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="11"/>
-      <c r="B172" s="11"/>
-      <c r="C172" s="11"/>
-      <c r="D172" s="11"/>
-      <c r="E172" s="11"/>
-      <c r="F172" s="11"/>
+      <c r="A172" s="7"/>
+      <c r="B172" s="7"/>
+      <c r="C172" s="7"/>
+      <c r="D172" s="7"/>
+      <c r="E172" s="7"/>
+      <c r="F172" s="7"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="A173" s="11"/>
-      <c r="B173" s="11"/>
-      <c r="C173" s="11"/>
-      <c r="D173" s="11"/>
-      <c r="E173" s="11"/>
-      <c r="F173" s="11"/>
+      <c r="A173" s="7"/>
+      <c r="B173" s="7"/>
+      <c r="C173" s="7"/>
+      <c r="D173" s="7"/>
+      <c r="E173" s="7"/>
+      <c r="F173" s="7"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="11"/>
-      <c r="B174" s="11"/>
-      <c r="C174" s="11"/>
-      <c r="D174" s="11"/>
-      <c r="E174" s="11"/>
-      <c r="F174" s="11"/>
+      <c r="A174" s="7"/>
+      <c r="B174" s="7"/>
+      <c r="C174" s="7"/>
+      <c r="D174" s="7"/>
+      <c r="E174" s="7"/>
+      <c r="F174" s="7"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" s="11"/>
-      <c r="B175" s="11"/>
-      <c r="C175" s="11"/>
-      <c r="D175" s="11"/>
-      <c r="E175" s="11"/>
-      <c r="F175" s="11"/>
+      <c r="A175" s="7"/>
+      <c r="B175" s="7"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7"/>
+      <c r="F175" s="7"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="11"/>
-      <c r="B176" s="11"/>
-      <c r="C176" s="11"/>
-      <c r="D176" s="11"/>
-      <c r="E176" s="11"/>
-      <c r="F176" s="11"/>
+      <c r="A176" s="7"/>
+      <c r="B176" s="7"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="11"/>
-      <c r="B177" s="11"/>
-      <c r="C177" s="11"/>
-      <c r="D177" s="11"/>
-      <c r="E177" s="11"/>
-      <c r="F177" s="11"/>
+      <c r="A177" s="7"/>
+      <c r="B177" s="7"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="7"/>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="11"/>
-      <c r="B178" s="11"/>
-      <c r="C178" s="11"/>
-      <c r="D178" s="11"/>
-      <c r="E178" s="11"/>
-      <c r="F178" s="11"/>
+      <c r="A178" s="7"/>
+      <c r="B178" s="7"/>
+      <c r="C178" s="7"/>
+      <c r="D178" s="7"/>
+      <c r="E178" s="7"/>
+      <c r="F178" s="7"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
-      <c r="A179" s="11"/>
-      <c r="B179" s="11"/>
-      <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
-      <c r="E179" s="11"/>
-      <c r="F179" s="11"/>
+      <c r="A179" s="7"/>
+      <c r="B179" s="7"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="7"/>
+      <c r="F179" s="7"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="11"/>
-      <c r="B180" s="11"/>
-      <c r="C180" s="11"/>
-      <c r="D180" s="11"/>
-      <c r="E180" s="11"/>
-      <c r="F180" s="11"/>
+      <c r="A180" s="7"/>
+      <c r="B180" s="7"/>
+      <c r="C180" s="7"/>
+      <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
+      <c r="F180" s="7"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="11"/>
-      <c r="B181" s="11"/>
-      <c r="C181" s="11"/>
-      <c r="D181" s="11"/>
-      <c r="E181" s="11"/>
-      <c r="F181" s="11"/>
+      <c r="A181" s="7"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="A182" s="11"/>
-      <c r="B182" s="11"/>
-      <c r="C182" s="11"/>
-      <c r="D182" s="11"/>
-      <c r="E182" s="11"/>
-      <c r="F182" s="11"/>
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="A183" s="11"/>
-      <c r="B183" s="11"/>
-      <c r="C183" s="11"/>
-      <c r="D183" s="11"/>
-      <c r="E183" s="11"/>
-      <c r="F183" s="11"/>
+      <c r="A183" s="7"/>
+      <c r="B183" s="7"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="A184" s="11"/>
-      <c r="B184" s="11"/>
-      <c r="C184" s="11"/>
-      <c r="D184" s="11"/>
-      <c r="E184" s="11"/>
-      <c r="F184" s="11"/>
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="7"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7"/>
+      <c r="F184" s="7"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="A185" s="11"/>
-      <c r="B185" s="11"/>
-      <c r="C185" s="11"/>
-      <c r="D185" s="11"/>
-      <c r="E185" s="11"/>
-      <c r="F185" s="11"/>
+      <c r="A185" s="7"/>
+      <c r="B185" s="7"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7"/>
+      <c r="F185" s="7"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="A186" s="11"/>
-      <c r="B186" s="11"/>
-      <c r="C186" s="11"/>
-      <c r="D186" s="11"/>
-      <c r="E186" s="11"/>
-      <c r="F186" s="11"/>
+      <c r="A186" s="7"/>
+      <c r="B186" s="7"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="7"/>
+      <c r="F186" s="7"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
-      <c r="A187" s="11"/>
-      <c r="B187" s="11"/>
-      <c r="C187" s="11"/>
-      <c r="D187" s="11"/>
-      <c r="E187" s="11"/>
-      <c r="F187" s="11"/>
+      <c r="A187" s="7"/>
+      <c r="B187" s="7"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="11"/>
-      <c r="B188" s="11"/>
-      <c r="C188" s="11"/>
-      <c r="D188" s="11"/>
-      <c r="E188" s="11"/>
-      <c r="F188" s="11"/>
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" s="11"/>
-      <c r="B189" s="11"/>
-      <c r="C189" s="11"/>
-      <c r="D189" s="11"/>
-      <c r="E189" s="11"/>
-      <c r="F189" s="11"/>
+      <c r="A189" s="7"/>
+      <c r="B189" s="7"/>
+      <c r="C189" s="7"/>
+      <c r="D189" s="7"/>
+      <c r="E189" s="7"/>
+      <c r="F189" s="7"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" s="11"/>
-      <c r="B190" s="11"/>
-      <c r="C190" s="11"/>
-      <c r="D190" s="11"/>
-      <c r="E190" s="11"/>
-      <c r="F190" s="11"/>
+      <c r="A190" s="7"/>
+      <c r="B190" s="7"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="7"/>
+      <c r="F190" s="7"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="A191" s="11"/>
-      <c r="B191" s="11"/>
-      <c r="C191" s="11"/>
-      <c r="D191" s="11"/>
-      <c r="E191" s="11"/>
-      <c r="F191" s="11"/>
+      <c r="A191" s="7"/>
+      <c r="B191" s="7"/>
+      <c r="C191" s="7"/>
+      <c r="D191" s="7"/>
+      <c r="E191" s="7"/>
+      <c r="F191" s="7"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" s="11"/>
-      <c r="B192" s="11"/>
-      <c r="C192" s="11"/>
-      <c r="D192" s="11"/>
-      <c r="E192" s="11"/>
-      <c r="F192" s="11"/>
+      <c r="A192" s="7"/>
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
-      <c r="A193" s="11"/>
-      <c r="B193" s="11"/>
-      <c r="C193" s="11"/>
-      <c r="D193" s="11"/>
-      <c r="E193" s="11"/>
-      <c r="F193" s="11"/>
+      <c r="A193" s="7"/>
+      <c r="B193" s="7"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="7"/>
+      <c r="E193" s="7"/>
+      <c r="F193" s="7"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="A194" s="11"/>
-      <c r="B194" s="11"/>
-      <c r="C194" s="11"/>
-      <c r="D194" s="11"/>
-      <c r="E194" s="11"/>
-      <c r="F194" s="11"/>
+      <c r="A194" s="7"/>
+      <c r="B194" s="7"/>
+      <c r="C194" s="7"/>
+      <c r="D194" s="7"/>
+      <c r="E194" s="7"/>
+      <c r="F194" s="7"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="A195" s="11"/>
-      <c r="B195" s="11"/>
-      <c r="C195" s="11"/>
-      <c r="D195" s="11"/>
-      <c r="E195" s="11"/>
-      <c r="F195" s="11"/>
+      <c r="A195" s="7"/>
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7"/>
+      <c r="F195" s="7"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="A196" s="11"/>
-      <c r="B196" s="11"/>
-      <c r="C196" s="11"/>
-      <c r="D196" s="11"/>
-      <c r="E196" s="11"/>
-      <c r="F196" s="11"/>
+      <c r="A196" s="7"/>
+      <c r="B196" s="7"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="7"/>
+      <c r="F196" s="7"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="A197" s="11"/>
-      <c r="B197" s="11"/>
-      <c r="C197" s="11"/>
-      <c r="D197" s="11"/>
-      <c r="E197" s="11"/>
-      <c r="F197" s="11"/>
+      <c r="A197" s="7"/>
+      <c r="B197" s="7"/>
+      <c r="C197" s="7"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="7"/>
+      <c r="F197" s="7"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="A198" s="11"/>
-      <c r="B198" s="11"/>
-      <c r="C198" s="11"/>
-      <c r="D198" s="11"/>
-      <c r="E198" s="11"/>
-      <c r="F198" s="11"/>
+      <c r="A198" s="7"/>
+      <c r="B198" s="7"/>
+      <c r="C198" s="7"/>
+      <c r="D198" s="7"/>
+      <c r="E198" s="7"/>
+      <c r="F198" s="7"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="A199" s="11"/>
-      <c r="B199" s="11"/>
-      <c r="C199" s="11"/>
-      <c r="D199" s="11"/>
-      <c r="E199" s="11"/>
-      <c r="F199" s="11"/>
+      <c r="A199" s="7"/>
+      <c r="B199" s="7"/>
+      <c r="C199" s="7"/>
+      <c r="D199" s="7"/>
+      <c r="E199" s="7"/>
+      <c r="F199" s="7"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
-      <c r="A200" s="11"/>
-      <c r="B200" s="11"/>
-      <c r="C200" s="11"/>
-      <c r="D200" s="11"/>
-      <c r="E200" s="11"/>
-      <c r="F200" s="11"/>
+      <c r="A200" s="7"/>
+      <c r="B200" s="7"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="7"/>
+      <c r="E200" s="7"/>
+      <c r="F200" s="7"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
-      <c r="A201" s="11"/>
-      <c r="B201" s="11"/>
-      <c r="C201" s="11"/>
-      <c r="D201" s="11"/>
-      <c r="E201" s="11"/>
-      <c r="F201" s="11"/>
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
+      <c r="C201" s="7"/>
+      <c r="D201" s="7"/>
+      <c r="E201" s="7"/>
+      <c r="F201" s="7"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
-      <c r="A202" s="11"/>
-      <c r="B202" s="11"/>
-      <c r="C202" s="11"/>
-      <c r="D202" s="11"/>
-      <c r="E202" s="11"/>
-      <c r="F202" s="11"/>
+      <c r="A202" s="7"/>
+      <c r="B202" s="7"/>
+      <c r="C202" s="7"/>
+      <c r="D202" s="7"/>
+      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
-      <c r="A203" s="11"/>
-      <c r="B203" s="11"/>
-      <c r="C203" s="11"/>
-      <c r="D203" s="11"/>
-      <c r="E203" s="11"/>
-      <c r="F203" s="11"/>
+      <c r="A203" s="7"/>
+      <c r="B203" s="7"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="7"/>
+      <c r="E203" s="7"/>
+      <c r="F203" s="7"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
-      <c r="A204" s="11"/>
-      <c r="B204" s="11"/>
-      <c r="C204" s="11"/>
-      <c r="D204" s="11"/>
-      <c r="E204" s="11"/>
-      <c r="F204" s="11"/>
+      <c r="A204" s="7"/>
+      <c r="B204" s="7"/>
+      <c r="C204" s="7"/>
+      <c r="D204" s="7"/>
+      <c r="E204" s="7"/>
+      <c r="F204" s="7"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="A205" s="11"/>
-      <c r="B205" s="11"/>
-      <c r="C205" s="11"/>
-      <c r="D205" s="11"/>
-      <c r="E205" s="11"/>
-      <c r="F205" s="11"/>
+      <c r="A205" s="7"/>
+      <c r="B205" s="7"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="A206" s="11"/>
-      <c r="B206" s="11"/>
-      <c r="C206" s="11"/>
-      <c r="D206" s="11"/>
-      <c r="E206" s="11"/>
-      <c r="F206" s="11"/>
+      <c r="A206" s="7"/>
+      <c r="B206" s="7"/>
+      <c r="C206" s="7"/>
+      <c r="D206" s="7"/>
+      <c r="E206" s="7"/>
+      <c r="F206" s="7"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="A207" s="11"/>
-      <c r="B207" s="11"/>
-      <c r="C207" s="11"/>
-      <c r="D207" s="11"/>
-      <c r="E207" s="11"/>
-      <c r="F207" s="11"/>
+      <c r="A207" s="7"/>
+      <c r="B207" s="7"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="7"/>
+      <c r="E207" s="7"/>
+      <c r="F207" s="7"/>
     </row>
     <row r="208" ht="14.25" customHeight="1">
-      <c r="A208" s="11"/>
-      <c r="B208" s="11"/>
-      <c r="C208" s="11"/>
-      <c r="D208" s="11"/>
-      <c r="E208" s="11"/>
-      <c r="F208" s="11"/>
+      <c r="A208" s="7"/>
+      <c r="B208" s="7"/>
+      <c r="C208" s="7"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="7"/>
+      <c r="F208" s="7"/>
     </row>
     <row r="209" ht="14.25" customHeight="1">
-      <c r="A209" s="11"/>
-      <c r="B209" s="11"/>
-      <c r="C209" s="11"/>
-      <c r="D209" s="11"/>
-      <c r="E209" s="11"/>
-      <c r="F209" s="11"/>
+      <c r="A209" s="7"/>
+      <c r="B209" s="7"/>
+      <c r="C209" s="7"/>
+      <c r="D209" s="7"/>
+      <c r="E209" s="7"/>
+      <c r="F209" s="7"/>
     </row>
     <row r="210" ht="14.25" customHeight="1">
-      <c r="A210" s="11"/>
-      <c r="B210" s="11"/>
-      <c r="C210" s="11"/>
-      <c r="D210" s="11"/>
-      <c r="E210" s="11"/>
-      <c r="F210" s="11"/>
+      <c r="A210" s="7"/>
+      <c r="B210" s="7"/>
+      <c r="C210" s="7"/>
+      <c r="D210" s="7"/>
+      <c r="E210" s="7"/>
+      <c r="F210" s="7"/>
     </row>
     <row r="211" ht="14.25" customHeight="1">
-      <c r="A211" s="11"/>
-      <c r="B211" s="11"/>
-      <c r="C211" s="11"/>
-      <c r="D211" s="11"/>
-      <c r="E211" s="11"/>
-      <c r="F211" s="11"/>
+      <c r="A211" s="7"/>
+      <c r="B211" s="7"/>
+      <c r="C211" s="7"/>
+      <c r="D211" s="7"/>
+      <c r="E211" s="7"/>
+      <c r="F211" s="7"/>
     </row>
     <row r="212" ht="14.25" customHeight="1">
-      <c r="A212" s="11"/>
-      <c r="B212" s="11"/>
-      <c r="C212" s="11"/>
-      <c r="D212" s="11"/>
-      <c r="E212" s="11"/>
-      <c r="F212" s="11"/>
+      <c r="A212" s="7"/>
+      <c r="B212" s="7"/>
+      <c r="C212" s="7"/>
+      <c r="D212" s="7"/>
+      <c r="E212" s="7"/>
+      <c r="F212" s="7"/>
     </row>
     <row r="213" ht="14.25" customHeight="1">
-      <c r="A213" s="11"/>
-      <c r="B213" s="11"/>
-      <c r="C213" s="11"/>
-      <c r="D213" s="11"/>
-      <c r="E213" s="11"/>
-      <c r="F213" s="11"/>
+      <c r="A213" s="7"/>
+      <c r="B213" s="7"/>
+      <c r="C213" s="7"/>
+      <c r="D213" s="7"/>
+      <c r="E213" s="7"/>
+      <c r="F213" s="7"/>
     </row>
     <row r="214" ht="14.25" customHeight="1">
-      <c r="A214" s="11"/>
-      <c r="B214" s="11"/>
-      <c r="C214" s="11"/>
-      <c r="D214" s="11"/>
-      <c r="E214" s="11"/>
-      <c r="F214" s="11"/>
-    </row>
-    <row r="215" ht="14.25" customHeight="1">
-      <c r="A215" s="11"/>
-      <c r="B215" s="11"/>
-      <c r="C215" s="11"/>
-      <c r="D215" s="11"/>
-      <c r="E215" s="11"/>
-      <c r="F215" s="11"/>
-    </row>
-    <row r="216" ht="14.25" customHeight="1">
-      <c r="A216" s="11"/>
-      <c r="B216" s="11"/>
-      <c r="C216" s="11"/>
-      <c r="D216" s="11"/>
-      <c r="E216" s="11"/>
-      <c r="F216" s="11"/>
-    </row>
-    <row r="217" ht="14.25" customHeight="1">
-      <c r="A217" s="11"/>
-      <c r="B217" s="11"/>
-      <c r="C217" s="11"/>
-      <c r="D217" s="11"/>
-      <c r="E217" s="11"/>
-      <c r="F217" s="11"/>
-    </row>
+      <c r="A214" s="7"/>
+      <c r="B214" s="7"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="7"/>
+      <c r="E214" s="7"/>
+      <c r="F214" s="7"/>
+    </row>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
     <row r="218" ht="14.25" customHeight="1"/>
     <row r="219" ht="14.25" customHeight="1"/>
     <row r="220" ht="14.25" customHeight="1"/>
@@ -3051,13 +2991,7 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.5" footer="0.0" header="0.0" left="0.7" right="0.45" top="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>